<commit_message>
minor optimizations to testing
</commit_message>
<xml_diff>
--- a/torch_eval/esg_model/classification_report.xlsx
+++ b/torch_eval/esg_model/classification_report.xlsx
@@ -435,13 +435,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.7745098039215687</v>
+        <v>0.7570093457943925</v>
       </c>
       <c r="C2">
-        <v>0.572463768115942</v>
+        <v>0.5869565217391305</v>
       </c>
       <c r="D2">
-        <v>0.6583333333333333</v>
+        <v>0.6612244897959184</v>
       </c>
       <c r="E2">
         <v>138</v>
@@ -452,13 +452,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.6835164835164835</v>
+        <v>0.6846846846846847</v>
       </c>
       <c r="C3">
-        <v>0.7641277641277642</v>
+        <v>0.7469287469287469</v>
       </c>
       <c r="D3">
-        <v>0.7215777262180975</v>
+        <v>0.7144535840188014</v>
       </c>
       <c r="E3">
         <v>407</v>
@@ -469,13 +469,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.7560975609756098</v>
+        <v>0.7453874538745388</v>
       </c>
       <c r="C4">
-        <v>0.7603773584905661</v>
+        <v>0.7622641509433963</v>
       </c>
       <c r="D4">
-        <v>0.7582314205079964</v>
+        <v>0.7537313432835822</v>
       </c>
       <c r="E4">
         <v>530</v>
@@ -486,13 +486,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.6956521739130435</v>
+        <v>0.7429718875502008</v>
       </c>
       <c r="C5">
-        <v>0.6423357664233577</v>
+        <v>0.6751824817518248</v>
       </c>
       <c r="D5">
-        <v>0.667931688804554</v>
+        <v>0.7074569789674952</v>
       </c>
       <c r="E5">
         <v>274</v>
@@ -503,13 +503,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0.6352941176470588</v>
+        <v>0.659217877094972</v>
       </c>
       <c r="C6">
-        <v>0.6242774566473989</v>
+        <v>0.6820809248554913</v>
       </c>
       <c r="D6">
-        <v>0.6297376093294461</v>
+        <v>0.6704545454545453</v>
       </c>
       <c r="E6">
         <v>173</v>
@@ -520,13 +520,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>0.631578947368421</v>
+        <v>0.6938775510204082</v>
       </c>
       <c r="C7">
-        <v>0.75</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="D7">
-        <v>0.6857142857142857</v>
+        <v>0.7010309278350516</v>
       </c>
       <c r="E7">
         <v>48</v>
@@ -537,13 +537,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>0.7089171974522293</v>
+        <v>0.7171974522292993</v>
       </c>
       <c r="C8">
-        <v>0.7089171974522293</v>
+        <v>0.7171974522292993</v>
       </c>
       <c r="D8">
-        <v>0.7089171974522293</v>
+        <v>0.7171974522292993</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -554,13 +554,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>0.6961081812236976</v>
+        <v>0.7138581333365329</v>
       </c>
       <c r="C9">
-        <v>0.6855970189675048</v>
+        <v>0.6936243599253205</v>
       </c>
       <c r="D9">
-        <v>0.6869210106512855</v>
+        <v>0.701391978225899</v>
       </c>
       <c r="E9">
         <v>1570</v>
@@ -571,13 +571,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>0.7112328895084444</v>
+        <v>0.7191811587993395</v>
       </c>
       <c r="C10">
-        <v>0.7089171974522293</v>
+        <v>0.7171974522292993</v>
       </c>
       <c r="D10">
-        <v>0.7078133517839054</v>
+        <v>0.7165544798500637</v>
       </c>
       <c r="E10">
         <v>1570</v>

</xml_diff>